<commit_message>
Refining Epsilon Search strategy, paths still seem too long for a greedy bias in the search
</commit_message>
<xml_diff>
--- a/examples/gridworld/TestRigs/qv-analysis.xlsx
+++ b/examples/gridworld/TestRigs/qv-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\devroot\ML\TicTacToe-DeepLearning\examples\gridworld\TestRigs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F64C0F6-4D76-4F37-B8DB-40B9EA5223A0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7204962C-DD94-4342-A311-F7F6A4770D81}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25785" windowHeight="13965" activeTab="1"/>
   </bookViews>
@@ -352,7 +352,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2906,8 +2906,8 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="20"/>
-      <c:rotY val="170"/>
+      <c:rotX val="10"/>
+      <c:rotY val="80"/>
       <c:rAngAx val="0"/>
     </c:view3D>
     <c:floor>
@@ -4949,7 +4949,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="r"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -13205,8 +13205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="W103" sqref="W103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19635,11 +19635,11 @@
     </row>
     <row r="92" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="str">
-        <f>IF(B71=B47,"^",IF(B71=C48,"&gt;",IF(B71=B49,"v",IF(B71=A48,"&lt;","?"))))</f>
+        <f t="shared" ref="B92:U92" si="28">IF(MAX(B47,C48,B49,A48)=B47,"^",IF(MAX(B47,C48,B49,A48)=C48,"&gt;",IF(MAX(B47,C48,B49,A48)=B49,"v",IF(MAX(B47,C48,B49,A48)=A48,"&lt;","?"))))</f>
         <v>&gt;</v>
       </c>
       <c r="C92" s="4" t="str">
-        <f t="shared" ref="C92:U92" si="28">IF(C71=C47,"^",IF(C71=D48,"&gt;",IF(C71=C49,"v",IF(C71=B48,"&lt;","?"))))</f>
+        <f t="shared" si="28"/>
         <v>&gt;</v>
       </c>
       <c r="D92" s="4" t="str">
@@ -19717,7 +19717,7 @@
     </row>
     <row r="93" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="str">
-        <f t="shared" ref="B93:U105" si="29">IF(B72=B48,"^",IF(B72=C49,"&gt;",IF(B72=B50,"v",IF(B72=A49,"&lt;","?"))))</f>
+        <f t="shared" ref="B93:U93" si="29">IF(MAX(B48,C49,B50,A49)=B48,"^",IF(MAX(B48,C49,B50,A49)=C49,"&gt;",IF(MAX(B48,C49,B50,A49)=B50,"v",IF(MAX(B48,C49,B50,A49)=A49,"&lt;","?"))))</f>
         <v>&gt;</v>
       </c>
       <c r="C93" s="4" t="str">
@@ -19799,1477 +19799,1477 @@
     </row>
     <row r="94" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B94:U94" si="30">IF(MAX(B49,C50,B51,A50)=B49,"^",IF(MAX(B49,C50,B51,A50)=C50,"&gt;",IF(MAX(B49,C50,B51,A50)=B51,"v",IF(MAX(B49,C50,B51,A50)=A50,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="D94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>^</v>
       </c>
       <c r="E94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="F94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>&gt;</v>
       </c>
       <c r="G94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="H94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="I94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="J94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="K94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="L94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="M94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>^</v>
       </c>
       <c r="N94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>^</v>
       </c>
       <c r="O94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>^</v>
       </c>
       <c r="P94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>&lt;</v>
       </c>
       <c r="Q94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>&lt;</v>
       </c>
       <c r="R94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>v</v>
       </c>
       <c r="S94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>^</v>
       </c>
       <c r="T94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>&lt;</v>
       </c>
       <c r="U94" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>&lt;</v>
       </c>
     </row>
     <row r="95" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B95:U95" si="31">IF(MAX(B50,C51,B52,A51)=B50,"^",IF(MAX(B50,C51,B52,A51)=C51,"&gt;",IF(MAX(B50,C51,B52,A51)=B52,"v",IF(MAX(B50,C51,B52,A51)=A51,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="D95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&gt;</v>
       </c>
       <c r="E95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="F95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&gt;</v>
       </c>
       <c r="G95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="H95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="I95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="J95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>v</v>
       </c>
       <c r="K95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&gt;</v>
       </c>
       <c r="L95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&lt;</v>
       </c>
       <c r="M95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&lt;</v>
       </c>
       <c r="N95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>^</v>
       </c>
       <c r="O95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>^</v>
       </c>
       <c r="P95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&lt;</v>
       </c>
       <c r="Q95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&gt;</v>
       </c>
       <c r="R95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>^</v>
       </c>
       <c r="S95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>&lt;</v>
       </c>
       <c r="T95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>^</v>
       </c>
       <c r="U95" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>^</v>
       </c>
     </row>
     <row r="96" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B96:U96" si="32">IF(MAX(B51,C52,B53,A52)=B51,"^",IF(MAX(B51,C52,B53,A52)=C52,"&gt;",IF(MAX(B51,C52,B53,A52)=B53,"v",IF(MAX(B51,C52,B53,A52)=A52,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="D96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>&lt;</v>
       </c>
       <c r="E96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="F96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="G96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="H96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="I96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>&lt;</v>
       </c>
       <c r="J96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>v</v>
       </c>
       <c r="K96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>&lt;</v>
       </c>
       <c r="L96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="M96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>&lt;</v>
       </c>
       <c r="N96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="O96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="P96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="Q96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>&lt;</v>
       </c>
       <c r="R96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="S96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="T96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
       <c r="U96" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>^</v>
       </c>
     </row>
     <row r="97" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B97:U97" si="33">IF(MAX(B52,C53,B54,A53)=B52,"^",IF(MAX(B52,C53,B54,A53)=C53,"&gt;",IF(MAX(B52,C53,B54,A53)=B54,"v",IF(MAX(B52,C53,B54,A53)=A53,"&lt;","?"))))</f>
         <v>&gt;</v>
       </c>
       <c r="C97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="D97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="E97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&gt;</v>
       </c>
       <c r="F97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&gt;</v>
       </c>
       <c r="G97" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>v</v>
       </c>
       <c r="H97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="I97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="J97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="K97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="L97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
       <c r="M97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="N97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="O97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&gt;</v>
       </c>
       <c r="P97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
       <c r="Q97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
       <c r="R97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
       <c r="S97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>&lt;</v>
       </c>
       <c r="T97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
       <c r="U97" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>^</v>
       </c>
     </row>
     <row r="98" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B98:U98" si="34">IF(MAX(B53,C54,B55,A54)=B53,"^",IF(MAX(B53,C54,B55,A54)=C54,"&gt;",IF(MAX(B53,C54,B55,A54)=B55,"v",IF(MAX(B53,C54,B55,A54)=A54,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="D98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="E98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&gt;</v>
       </c>
       <c r="F98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&gt;</v>
       </c>
       <c r="G98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="H98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="I98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="J98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="K98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="L98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="M98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="N98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="O98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="P98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="Q98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="R98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="S98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>&lt;</v>
       </c>
       <c r="T98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
       <c r="U98" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>^</v>
       </c>
     </row>
     <row r="99" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B99:U99" si="35">IF(MAX(B54,C55,B56,A55)=B54,"^",IF(MAX(B54,C55,B56,A55)=C55,"&gt;",IF(MAX(B54,C55,B56,A55)=B56,"v",IF(MAX(B54,C55,B56,A55)=A55,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="D99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="E99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&gt;</v>
       </c>
       <c r="F99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="G99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="H99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="I99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="J99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="K99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="L99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="M99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="N99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="O99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>&lt;</v>
       </c>
       <c r="P99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="Q99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="R99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="S99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="T99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
       <c r="U99" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>^</v>
       </c>
     </row>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B100:U100" si="36">IF(MAX(B55,C56,B57,A56)=B55,"^",IF(MAX(B55,C56,B57,A56)=C56,"&gt;",IF(MAX(B55,C56,B57,A56)=B57,"v",IF(MAX(B55,C56,B57,A56)=A56,"&lt;","?"))))</f>
         <v>&gt;</v>
       </c>
       <c r="C100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>v</v>
       </c>
       <c r="D100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="E100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="F100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="G100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="H100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="I100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>&lt;</v>
       </c>
       <c r="J100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="K100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="L100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>&lt;</v>
       </c>
       <c r="M100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="N100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="O100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="P100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="Q100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="R100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="S100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="T100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
       <c r="U100" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>^</v>
       </c>
     </row>
     <row r="101" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B101:U101" si="37">IF(MAX(B56,C57,B58,A57)=B56,"^",IF(MAX(B56,C57,B58,A57)=C57,"&gt;",IF(MAX(B56,C57,B58,A57)=B58,"v",IF(MAX(B56,C57,B58,A57)=A57,"&lt;","?"))))</f>
         <v>&gt;</v>
       </c>
       <c r="C101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>v</v>
       </c>
       <c r="D101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>&lt;</v>
       </c>
       <c r="E101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>&lt;</v>
       </c>
       <c r="F101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>v</v>
       </c>
       <c r="G101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>&lt;</v>
       </c>
       <c r="H101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="I101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="J101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="K101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="L101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="M101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="N101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="O101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>&lt;</v>
       </c>
       <c r="P101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="Q101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="R101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="S101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="T101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
       <c r="U101" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>^</v>
       </c>
     </row>
     <row r="102" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B102:U102" si="38">IF(MAX(B57,C58,B59,A58)=B57,"^",IF(MAX(B57,C58,B59,A58)=C58,"&gt;",IF(MAX(B57,C58,B59,A58)=B59,"v",IF(MAX(B57,C58,B59,A58)=A58,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="D102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="E102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>v</v>
       </c>
       <c r="F102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="G102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="H102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="I102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="J102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="K102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="L102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="M102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="N102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="O102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="P102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="Q102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>&lt;</v>
       </c>
       <c r="R102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="S102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="T102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
       <c r="U102" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>^</v>
       </c>
     </row>
     <row r="103" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B103:U103" si="39">IF(MAX(B58,C59,B60,A59)=B58,"^",IF(MAX(B58,C59,B60,A59)=C59,"&gt;",IF(MAX(B58,C59,B60,A59)=B60,"v",IF(MAX(B58,C59,B60,A59)=A59,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="D103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>v</v>
       </c>
       <c r="E103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="F103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="G103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>v</v>
       </c>
       <c r="H103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="I103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="J103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="K103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="L103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="M103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="N103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="O103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="P103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="Q103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>&lt;</v>
       </c>
       <c r="R103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="S103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="T103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
       <c r="U103" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="39"/>
         <v>^</v>
       </c>
     </row>
     <row r="104" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B104:U104" si="40">IF(MAX(B59,C60,B61,A60)=B59,"^",IF(MAX(B59,C60,B61,A60)=C60,"&gt;",IF(MAX(B59,C60,B61,A60)=B61,"v",IF(MAX(B59,C60,B61,A60)=A60,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&gt;</v>
       </c>
       <c r="D104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>v</v>
       </c>
       <c r="E104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="F104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>v</v>
       </c>
       <c r="G104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="H104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="I104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="J104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="K104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="L104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="M104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="N104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>&lt;</v>
       </c>
       <c r="O104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="P104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="Q104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="R104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="S104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="T104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
       <c r="U104" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v>^</v>
       </c>
     </row>
     <row r="105" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="B105:U105" si="41">IF(MAX(B60,C61,B62,A61)=B60,"^",IF(MAX(B60,C61,B62,A61)=C61,"&gt;",IF(MAX(B60,C61,B62,A61)=B62,"v",IF(MAX(B60,C61,B62,A61)=A61,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&gt;</v>
       </c>
       <c r="D105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>^</v>
       </c>
       <c r="E105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="F105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="G105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="H105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="I105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="J105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="K105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="L105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="M105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="N105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="O105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="P105" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="Q105" s="4" t="str">
-        <f t="shared" ref="Q105:AJ105" si="30">IF(Q84=Q60,"^",IF(Q84=R61,"&gt;",IF(Q84=Q62,"v",IF(Q84=P61,"&lt;","?"))))</f>
+        <f t="shared" si="41"/>
         <v>v</v>
       </c>
       <c r="R105" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="41"/>
         <v>&lt;</v>
       </c>
       <c r="S105" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="41"/>
         <v>^</v>
       </c>
       <c r="T105" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="41"/>
         <v>^</v>
       </c>
       <c r="U105" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="41"/>
         <v>^</v>
       </c>
     </row>
     <row r="106" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="str">
-        <f t="shared" ref="B106:U111" si="31">IF(B85=B61,"^",IF(B85=C62,"&gt;",IF(B85=B63,"v",IF(B85=A62,"&lt;","?"))))</f>
+        <f t="shared" ref="B106:U106" si="42">IF(MAX(B61,C62,B63,A62)=B61,"^",IF(MAX(B61,C62,B63,A62)=C62,"&gt;",IF(MAX(B61,C62,B63,A62)=B63,"v",IF(MAX(B61,C62,B63,A62)=A62,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&gt;</v>
       </c>
       <c r="D106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="E106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="F106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="G106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="H106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>v</v>
       </c>
       <c r="I106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="J106" s="4" t="str">
-        <f>IF(J85=J61,"^",IF(J85=K62,"&gt;",IF(J85=J63,"v",IF(J85=I62,"&lt;","?"))))</f>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="K106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="L106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="M106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="N106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="O106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="P106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>v</v>
       </c>
       <c r="Q106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="R106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>&lt;</v>
       </c>
       <c r="S106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="T106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
       <c r="U106" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>^</v>
       </c>
     </row>
     <row r="107" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="B107:U107" si="43">IF(MAX(B62,C63,B64,A63)=B62,"^",IF(MAX(B62,C63,B64,A63)=C63,"&gt;",IF(MAX(B62,C63,B64,A63)=B64,"v",IF(MAX(B62,C63,B64,A63)=A63,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="D107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="E107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="F107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="G107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="H107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="I107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="J107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="K107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="L107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="M107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="N107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="O107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&gt;</v>
       </c>
       <c r="P107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="Q107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>v</v>
       </c>
       <c r="R107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="S107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>&lt;</v>
       </c>
       <c r="T107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
       <c r="U107" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v>^</v>
       </c>
     </row>
     <row r="108" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="B108:U108" si="44">IF(MAX(B63,C64,B65,A64)=B63,"^",IF(MAX(B63,C64,B65,A64)=C64,"&gt;",IF(MAX(B63,C64,B65,A64)=B65,"v",IF(MAX(B63,C64,B65,A64)=A64,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>v</v>
       </c>
       <c r="D108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="E108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="F108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="G108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="H108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="I108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="J108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>v</v>
       </c>
       <c r="K108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>v</v>
       </c>
       <c r="L108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="M108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="N108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="O108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="P108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&gt;</v>
       </c>
       <c r="Q108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="R108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>&lt;</v>
       </c>
       <c r="S108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="T108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
       <c r="U108" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="44"/>
         <v>^</v>
       </c>
     </row>
     <row r="109" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="B109:U109" si="45">IF(MAX(B64,C65,B66,A65)=B64,"^",IF(MAX(B64,C65,B66,A65)=C65,"&gt;",IF(MAX(B64,C65,B66,A65)=B66,"v",IF(MAX(B64,C65,B66,A65)=A65,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="D109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="E109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="F109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="G109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
       <c r="H109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
       <c r="I109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="J109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>v</v>
       </c>
       <c r="K109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="L109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="M109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="N109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="O109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="P109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="Q109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
       <c r="R109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>&lt;</v>
       </c>
       <c r="S109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
       <c r="T109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
       <c r="U109" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="45"/>
         <v>^</v>
       </c>
     </row>
     <row r="110" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="B110:U110" si="46">IF(MAX(B65,C66,B67,A66)=B65,"^",IF(MAX(B65,C66,B67,A66)=C66,"&gt;",IF(MAX(B65,C66,B67,A66)=B67,"v",IF(MAX(B65,C66,B67,A66)=A66,"&lt;","?"))))</f>
         <v>v</v>
       </c>
       <c r="C110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="D110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="E110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>v</v>
       </c>
       <c r="F110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="G110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="H110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="I110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>v</v>
       </c>
       <c r="J110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>v</v>
       </c>
       <c r="K110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="L110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="M110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="N110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="O110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="P110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="Q110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="R110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="S110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="T110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>&lt;</v>
       </c>
       <c r="U110" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>^</v>
       </c>
     </row>
     <row r="111" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="B111:U111" si="47">IF(MAX(B66,C67,B68,A67)=B66,"^",IF(MAX(B66,C67,B68,A67)=C67,"&gt;",IF(MAX(B66,C67,B68,A67)=B68,"v",IF(MAX(B66,C67,B68,A67)=A67,"&lt;","?"))))</f>
         <v>^</v>
       </c>
       <c r="C111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="D111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="E111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="F111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="G111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="H111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="I111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&gt;</v>
       </c>
       <c r="J111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="K111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="L111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="M111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="N111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="O111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="P111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="Q111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="R111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="S111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="T111" s="4" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>&lt;</v>
       </c>
       <c r="U111" s="4" t="str">
-        <f>IF(U90=U66,"^",IF(U90=V67,"&gt;",IF(U90=U68,"v",IF(U90=T67,"&lt;","?"))))</f>
+        <f>IF(MAX(U66,V67,U68,T67)=U66,"^",IF(MAX(U66,V67,U68,T67)=V67,"&gt;",IF(MAX(U66,V67,U68,T67)=U68,"v",IF(MAX(U66,V67,U68,T67)=T67,"&lt;","?"))))</f>
         <v>&lt;</v>
       </c>
     </row>

</xml_diff>